<commit_message>
Fix to intimate partner calcs
</commit_message>
<xml_diff>
--- a/data/excelsheets/nspintimatepartner.xlsx
+++ b/data/excelsheets/nspintimatepartner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>Table 3.5 of the NSP Survey 1995-2010</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Of people who had sex</t>
+  </si>
+  <si>
+    <t>SD Prop</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Difference calc</t>
   </si>
 </sst>
 </file>
@@ -403,13 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -453,7 +468,7 @@
         <v>307</v>
       </c>
       <c r="D5" s="1">
-        <f>C5/SUM(B5:C5)</f>
+        <f t="shared" ref="D5:D14" si="0">C5/SUM(B5:C5)</f>
         <v>0.75990099009900991</v>
       </c>
       <c r="F5" t="s">
@@ -472,7 +487,7 @@
         <v>357</v>
       </c>
       <c r="D6" s="1">
-        <f>C6/SUM(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>0.73608247422680417</v>
       </c>
       <c r="F6" s="1">
@@ -482,7 +497,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" ref="A7:A14" si="0">A6+1</f>
+        <f t="shared" ref="A7:A14" si="1">A6+1</f>
         <v>1997</v>
       </c>
       <c r="B7">
@@ -492,7 +507,7 @@
         <v>431</v>
       </c>
       <c r="D7" s="1">
-        <f>C7/SUM(B7:C7)</f>
+        <f t="shared" si="0"/>
         <v>0.63289280469897213</v>
       </c>
       <c r="F7" t="s">
@@ -501,7 +516,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1998</v>
       </c>
       <c r="B8">
@@ -511,7 +526,7 @@
         <v>637</v>
       </c>
       <c r="D8" s="1">
-        <f>C8/SUM(B8:C8)</f>
+        <f t="shared" si="0"/>
         <v>0.64408493427704749</v>
       </c>
       <c r="F8" s="1">
@@ -521,7 +536,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1999</v>
       </c>
       <c r="B9">
@@ -531,7 +546,7 @@
         <v>609</v>
       </c>
       <c r="D9" s="1">
-        <f>C9/SUM(B9:C9)</f>
+        <f t="shared" si="0"/>
         <v>0.67666666666666664</v>
       </c>
       <c r="F9" t="s">
@@ -540,7 +555,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="B10">
@@ -550,7 +565,7 @@
         <v>553</v>
       </c>
       <c r="D10" s="1">
-        <f>C10/SUM(B10:C10)</f>
+        <f t="shared" si="0"/>
         <v>0.61444444444444446</v>
       </c>
       <c r="F10" s="1">
@@ -560,7 +575,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2001</v>
       </c>
       <c r="B11">
@@ -570,7 +585,7 @@
         <v>448</v>
       </c>
       <c r="D11" s="1">
-        <f>C11/SUM(B11:C11)</f>
+        <f t="shared" si="0"/>
         <v>0.65979381443298968</v>
       </c>
       <c r="F11" t="s">
@@ -579,7 +594,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2002</v>
       </c>
       <c r="B12">
@@ -589,7 +604,7 @@
         <v>515</v>
       </c>
       <c r="D12" s="1">
-        <f>C12/SUM(B12:C12)</f>
+        <f t="shared" si="0"/>
         <v>0.69688768606224627</v>
       </c>
       <c r="F12" s="1">
@@ -599,7 +614,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2003</v>
       </c>
       <c r="B13">
@@ -609,7 +624,7 @@
         <v>558</v>
       </c>
       <c r="D13" s="1">
-        <f>C13/SUM(B13:C13)</f>
+        <f t="shared" si="0"/>
         <v>0.72093023255813948</v>
       </c>
       <c r="F13" t="s">
@@ -618,7 +633,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2004</v>
       </c>
       <c r="B14">
@@ -628,7 +643,7 @@
         <v>431</v>
       </c>
       <c r="D14" s="1">
-        <f>C14/SUM(B14:C14)</f>
+        <f t="shared" si="0"/>
         <v>0.67874015748031491</v>
       </c>
       <c r="F14" s="1">
@@ -654,7 +669,7 @@
         <v>4.6579725480238476E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>7</v>
       </c>
@@ -666,18 +681,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F18" s="1">
         <f>F12+F14+F16</f>
         <v>0.68204242049466346</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -690,8 +705,20 @@
       <c r="D20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2005</v>
       </c>
@@ -702,11 +729,21 @@
         <v>397</v>
       </c>
       <c r="D21" s="1">
-        <f>C21/SUM(B21:C21)</f>
+        <f t="shared" ref="D21:D26" si="2">C21/SUM(B21:C21)</f>
         <v>0.55836849507735586</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21">
+        <v>2005</v>
+      </c>
+      <c r="K21" s="1">
+        <f>D21+D33-$D$16</f>
+        <v>5.2879746899076596E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>A21+1</f>
         <v>2006</v>
@@ -718,13 +755,29 @@
         <v>376</v>
       </c>
       <c r="D22" s="1">
-        <f>C22/SUM(B22:C22)</f>
+        <f t="shared" si="2"/>
         <v>0.5662650602409639</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <f>F12/F4</f>
+        <v>0.74878822804756306</v>
+      </c>
+      <c r="G22">
+        <f>D30*F22</f>
+        <v>1.2921986889951843E-2</v>
+      </c>
+      <c r="J22">
+        <f>J21+1</f>
+        <v>2006</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" ref="K22:K32" si="3">D22+D34-$D$16</f>
+        <v>7.528581386032196E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ref="A23:A26" si="1">A22+1</f>
+        <f t="shared" ref="A23:A26" si="4">A22+1</f>
         <v>2007</v>
       </c>
       <c r="B23">
@@ -734,13 +787,24 @@
         <v>375</v>
       </c>
       <c r="D23" s="1">
-        <f>C23/SUM(B23:C23)</f>
+        <f t="shared" si="2"/>
         <v>0.55555555555555558</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:J26" si="5">J22+1</f>
+        <v>2007</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="3"/>
+        <v>2.276686640417569E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2008</v>
       </c>
       <c r="B24">
@@ -750,13 +814,29 @@
         <v>481</v>
       </c>
       <c r="D24" s="1">
-        <f>C24/SUM(B24:C24)</f>
+        <f t="shared" si="2"/>
         <v>0.55097365406643761</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <f>F14/F6</f>
+        <v>0.223866326688404</v>
+      </c>
+      <c r="G24">
+        <f>F24*D42</f>
+        <v>2.2388322524803165E-2</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>2008</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="3"/>
+        <v>5.8586405985567303E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2009</v>
       </c>
       <c r="B25">
@@ -766,13 +846,24 @@
         <v>439</v>
       </c>
       <c r="D25" s="1">
-        <f>C25/SUM(B25:C25)</f>
+        <f t="shared" si="2"/>
         <v>0.54331683168316836</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>2009</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="3"/>
+        <v>2.056644658673501E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
       <c r="B26">
@@ -782,11 +873,30 @@
         <v>370</v>
       </c>
       <c r="D26" s="1">
-        <f>C26/SUM(B26:C26)</f>
+        <f t="shared" si="2"/>
         <v>0.56923076923076921</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="1">
+        <f>F16/F4</f>
+        <v>6.82944697874594E-2</v>
+      </c>
+      <c r="G26">
+        <f>F26*K30</f>
+        <v>3.1168392076149548E-2</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>2010</v>
+      </c>
+      <c r="K26" s="1">
+        <f>D26+D38-$D$16</f>
+        <v>4.9393073145554633E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>6</v>
       </c>
@@ -794,8 +904,15 @@
         <f>AVERAGE(D21:D26)</f>
         <v>0.5572850609757084</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="1">
+        <f>AVERAGE(K21:K26)</f>
+        <v>4.6579725480238532E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>7</v>
       </c>
@@ -803,13 +920,37 @@
         <f>STDEV(D21:D26)</f>
         <v>9.6171787725229767E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29">
+        <f>STDEV(K21:K26)</f>
+        <v>2.1258165574543755E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <f>D29/D28</f>
+        <v>1.725719823833961E-2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30">
+        <f>K29/K28</f>
+        <v>0.45638237141527466</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -822,6 +963,7 @@
       <c r="D32" t="s">
         <v>5</v>
       </c>
+      <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -834,7 +976,7 @@
         <v>125</v>
       </c>
       <c r="D33" s="1">
-        <f>C33/SUM(B33:C33)</f>
+        <f t="shared" ref="D33:D38" si="6">C33/SUM(B33:C33)</f>
         <v>0.17655367231638419</v>
       </c>
     </row>
@@ -850,13 +992,13 @@
         <v>124</v>
       </c>
       <c r="D34" s="1">
-        <f>C34/SUM(B34:C34)</f>
+        <f t="shared" si="6"/>
         <v>0.19106317411402157</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" ref="A35:A38" si="2">A34+1</f>
+        <f t="shared" ref="A35:A38" si="7">A34+1</f>
         <v>2007</v>
       </c>
       <c r="B35">
@@ -866,13 +1008,13 @@
         <v>100</v>
       </c>
       <c r="D35" s="1">
-        <f>C35/SUM(B35:C35)</f>
+        <f t="shared" si="6"/>
         <v>0.14925373134328357</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2008</v>
       </c>
       <c r="B36">
@@ -882,13 +1024,13 @@
         <v>165</v>
       </c>
       <c r="D36" s="1">
-        <f>C36/SUM(B36:C36)</f>
+        <f t="shared" si="6"/>
         <v>0.18965517241379309</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2009</v>
       </c>
       <c r="B37">
@@ -898,13 +1040,13 @@
         <v>126</v>
       </c>
       <c r="D37" s="1">
-        <f>C37/SUM(B37:C37)</f>
+        <f t="shared" si="6"/>
         <v>0.15929203539823009</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2010</v>
       </c>
       <c r="B38">
@@ -914,7 +1056,7 @@
         <v>103</v>
       </c>
       <c r="D38" s="1">
-        <f>C38/SUM(B38:C38)</f>
+        <f t="shared" si="6"/>
         <v>0.16220472440944883</v>
       </c>
       <c r="F38" s="1"/>
@@ -935,6 +1077,15 @@
       <c r="D41">
         <f>STDEV(D33:D38)</f>
         <v>1.713500183866758E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <f>D41/D40</f>
+        <v>0.100007548504448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>